<commit_message>
atualização de processos do banco de dados
</commit_message>
<xml_diff>
--- a/backend/objetos.xlsx
+++ b/backend/objetos.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leozed92-my.sharepoint.com/personal/leozed_leozed92_onmicrosoft_com/Documents/Aplicativos/App GAD SESAU/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DEEE6D-2F43-435C-AC8E-A5B307752751}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8264AC03-D859-4ED8-9F5A-032729C3647F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
+    <workbookView xWindow="810" yWindow="2055" windowWidth="21600" windowHeight="11190" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="objetos" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">objetos!$A$1:$C$249</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="475">
   <si>
     <t>objeto</t>
   </si>
@@ -696,9 +699,6 @@
     <t>Contratação de empresa especializada em prestação de serviços de manutenção preventiva e corretiva, de forma continua, com fornecimento e reposição de peças, acessórios e componentes eletrônicos dos Sistemas de Climatização, de expansão indireta CHILLER com capacidade de 150 TR e 9,92 TR e de expansão direta através Condicionador de Ar Tipo Self Contained com Condensador a Ar Remoto de 7,5 TR, conforme dados técnicos em anexo, para atender o Hospital de Base Dr. Ary Pinheiro, por um período de 12 (doze) meses.</t>
   </si>
   <si>
-    <t>EMERGENCIAL</t>
-  </si>
-  <si>
     <t>0036.010175/2025-84</t>
   </si>
   <si>
@@ -717,9 +717,6 @@
     <t>Contratação de manutenção corretiva dos equipamentos Arco Cirúrgicos da marca VMI disponíveis na unidade Hospital de Base Dr. Ary Pinheiro</t>
   </si>
   <si>
-    <t>Licitatório - SRP</t>
-  </si>
-  <si>
     <t>Contratação, por Registro de Preço, de empresa(s) especializada(s) na prestação de serviços de Estudo Prévio/Análise, Adequação, Manutenção, Limpeza e Desinfecção em poços tubulares para atender às necessidades das unidades Laboratório Central de Saúde Pública - LACEN, Centro de Reabilitação de Rondônia - CERO, Assistência Médica Intensiva - AMI, Centro de Medicina Tropical de Rondônia - CEMETRON, Hospital Retaguarda de Rondônia - HRRO, Hospital Regional Cacoal - HRC, Hospital São Francisco do Guaporé - HRSFG, Hospital Regional de Extrema - HRE e Laboratório de Fronteira de Rondônia - LAFRON, por um período de 1 (um) ano, nos moldes da Lei Federal n.º 14.133 de 1º Abril de 2021.</t>
   </si>
   <si>
@@ -1465,6 +1462,9 @@
   </si>
   <si>
     <t>PRESERVAÇÃO DE ÓRGÃOS E CÓRNEAS</t>
+  </si>
+  <si>
+    <t>Licitatório SRP</t>
   </si>
 </sst>
 </file>
@@ -1506,9 +1506,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1850,7 +1851,7 @@
   <dimension ref="A1:C249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C25" sqref="C25:C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,37 +3012,37 @@
         <v>218</v>
       </c>
       <c r="C105" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>219</v>
+      </c>
+      <c r="B106" t="s">
         <v>220</v>
       </c>
-      <c r="B106" t="s">
-        <v>221</v>
-      </c>
       <c r="C106" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>221</v>
+      </c>
+      <c r="B107" t="s">
         <v>222</v>
       </c>
-      <c r="B107" t="s">
-        <v>223</v>
-      </c>
       <c r="C107" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>223</v>
+      </c>
+      <c r="B108" t="s">
         <v>224</v>
-      </c>
-      <c r="B108" t="s">
-        <v>225</v>
       </c>
       <c r="C108" t="s">
         <v>59</v>
@@ -3054,8 +3055,8 @@
       <c r="B109" t="s">
         <v>29</v>
       </c>
-      <c r="C109" t="s">
-        <v>226</v>
+      <c r="C109" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3065,8 +3066,8 @@
       <c r="B110" t="s">
         <v>65</v>
       </c>
-      <c r="C110" t="s">
-        <v>226</v>
+      <c r="C110" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3076,8 +3077,8 @@
       <c r="B111" t="s">
         <v>67</v>
       </c>
-      <c r="C111" t="s">
-        <v>226</v>
+      <c r="C111" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,8 +3088,8 @@
       <c r="B112" t="s">
         <v>87</v>
       </c>
-      <c r="C112" t="s">
-        <v>226</v>
+      <c r="C112" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3098,8 +3099,8 @@
       <c r="B113" t="s">
         <v>96</v>
       </c>
-      <c r="C113" t="s">
-        <v>226</v>
+      <c r="C113" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3109,8 +3110,8 @@
       <c r="B114" t="s">
         <v>106</v>
       </c>
-      <c r="C114" t="s">
-        <v>226</v>
+      <c r="C114" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3120,8 +3121,8 @@
       <c r="B115" t="s">
         <v>134</v>
       </c>
-      <c r="C115" t="s">
-        <v>226</v>
+      <c r="C115" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3131,8 +3132,8 @@
       <c r="B116" t="s">
         <v>140</v>
       </c>
-      <c r="C116" t="s">
-        <v>226</v>
+      <c r="C116" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3142,8 +3143,8 @@
       <c r="B117" t="s">
         <v>142</v>
       </c>
-      <c r="C117" t="s">
-        <v>226</v>
+      <c r="C117" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3153,8 +3154,8 @@
       <c r="B118" t="s">
         <v>147</v>
       </c>
-      <c r="C118" t="s">
-        <v>226</v>
+      <c r="C118" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3164,8 +3165,8 @@
       <c r="B119" t="s">
         <v>159</v>
       </c>
-      <c r="C119" t="s">
-        <v>226</v>
+      <c r="C119" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3173,10 +3174,10 @@
         <v>209</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
-      </c>
-      <c r="C120" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3186,16 +3187,16 @@
       <c r="B121" t="s">
         <v>85</v>
       </c>
-      <c r="C121" t="s">
-        <v>226</v>
+      <c r="C121" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B122" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C122" t="s">
         <v>23</v>
@@ -3203,10 +3204,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B123" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C123" t="s">
         <v>23</v>
@@ -3214,10 +3215,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B124" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C124" t="s">
         <v>23</v>
@@ -3225,10 +3226,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B125" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C125" t="s">
         <v>23</v>
@@ -3236,10 +3237,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B126" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C126" t="s">
         <v>23</v>
@@ -3247,10 +3248,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B127" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C127" t="s">
         <v>23</v>
@@ -3258,10 +3259,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C128" t="s">
         <v>23</v>
@@ -3272,7 +3273,7 @@
         <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C129" t="s">
         <v>23</v>
@@ -3283,7 +3284,7 @@
         <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C130" t="s">
         <v>23</v>
@@ -3291,10 +3292,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B131" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C131" t="s">
         <v>59</v>
@@ -3302,10 +3303,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C132" t="s">
         <v>70</v>
@@ -3313,10 +3314,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B133" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C133" t="s">
         <v>23</v>
@@ -3324,10 +3325,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B134" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C134" t="s">
         <v>59</v>
@@ -3338,7 +3339,7 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C135" t="s">
         <v>23</v>
@@ -3346,10 +3347,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B136" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C136" t="s">
         <v>23</v>
@@ -3357,10 +3358,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B137" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C137" t="s">
         <v>23</v>
@@ -3371,7 +3372,7 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C138" t="s">
         <v>23</v>
@@ -3382,7 +3383,7 @@
         <v>9</v>
       </c>
       <c r="B139" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C139" t="s">
         <v>23</v>
@@ -3390,10 +3391,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B140" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C140" t="s">
         <v>23</v>
@@ -3401,10 +3402,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B141" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C141" t="s">
         <v>70</v>
@@ -3412,10 +3413,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B142" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C142" t="s">
         <v>70</v>
@@ -3423,120 +3424,120 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
+        <v>263</v>
+      </c>
+      <c r="C143" t="s">
         <v>264</v>
-      </c>
-      <c r="B143" t="s">
-        <v>265</v>
-      </c>
-      <c r="C143" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B144" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C144" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B145" t="s">
-        <v>270</v>
-      </c>
-      <c r="C145" t="s">
-        <v>226</v>
+        <v>268</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B146" t="s">
-        <v>272</v>
-      </c>
-      <c r="C146" t="s">
-        <v>226</v>
+        <v>270</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B147" t="s">
-        <v>274</v>
-      </c>
-      <c r="C147" t="s">
-        <v>226</v>
+        <v>272</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B148" t="s">
-        <v>276</v>
-      </c>
-      <c r="C148" t="s">
-        <v>226</v>
+        <v>274</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B149" t="s">
-        <v>278</v>
-      </c>
-      <c r="C149" t="s">
-        <v>226</v>
+        <v>276</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B150" t="s">
-        <v>280</v>
-      </c>
-      <c r="C150" t="s">
-        <v>226</v>
+        <v>278</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B151" t="s">
-        <v>282</v>
-      </c>
-      <c r="C151" t="s">
-        <v>226</v>
+        <v>280</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B152" t="s">
-        <v>284</v>
-      </c>
-      <c r="C152" t="s">
-        <v>226</v>
+        <v>282</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B153" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C153" t="s">
         <v>43</v>
@@ -3544,32 +3545,32 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B154" t="s">
-        <v>288</v>
-      </c>
-      <c r="C154" t="s">
-        <v>226</v>
+        <v>286</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B155" t="s">
-        <v>290</v>
-      </c>
-      <c r="C155" t="s">
-        <v>226</v>
+        <v>288</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B156" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C156" t="s">
         <v>43</v>
@@ -3577,21 +3578,21 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B157" t="s">
-        <v>294</v>
-      </c>
-      <c r="C157" t="s">
-        <v>226</v>
+        <v>292</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B158" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C158" t="s">
         <v>23</v>
@@ -3599,32 +3600,32 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B159" t="s">
-        <v>298</v>
-      </c>
-      <c r="C159" t="s">
-        <v>226</v>
+        <v>296</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B160" t="s">
-        <v>300</v>
-      </c>
-      <c r="C160" t="s">
-        <v>226</v>
+        <v>298</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B161" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C161" t="s">
         <v>23</v>
@@ -3632,21 +3633,21 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B162" t="s">
-        <v>304</v>
-      </c>
-      <c r="C162" t="s">
-        <v>226</v>
+        <v>302</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B163" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C163" t="s">
         <v>23</v>
@@ -3654,54 +3655,54 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B164" t="s">
-        <v>308</v>
-      </c>
-      <c r="C164" t="s">
-        <v>226</v>
+        <v>306</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B165" t="s">
-        <v>310</v>
-      </c>
-      <c r="C165" t="s">
-        <v>226</v>
+        <v>308</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B166" t="s">
-        <v>312</v>
-      </c>
-      <c r="C166" t="s">
-        <v>226</v>
+        <v>310</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B167" t="s">
-        <v>314</v>
-      </c>
-      <c r="C167" t="s">
-        <v>226</v>
+        <v>312</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B168" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C168" t="s">
         <v>43</v>
@@ -3709,43 +3710,43 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B169" t="s">
-        <v>318</v>
-      </c>
-      <c r="C169" t="s">
-        <v>226</v>
+        <v>316</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B170" t="s">
-        <v>320</v>
-      </c>
-      <c r="C170" t="s">
-        <v>226</v>
+        <v>318</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B171" t="s">
-        <v>322</v>
-      </c>
-      <c r="C171" t="s">
-        <v>226</v>
+        <v>320</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B172" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C172" t="s">
         <v>23</v>
@@ -3753,10 +3754,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B173" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C173" t="s">
         <v>23</v>
@@ -3764,10 +3765,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B174" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C174" t="s">
         <v>43</v>
@@ -3775,10 +3776,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B175" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C175" t="s">
         <v>43</v>
@@ -3786,10 +3787,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B176" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C176" t="s">
         <v>23</v>
@@ -3797,32 +3798,32 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B177" t="s">
-        <v>334</v>
-      </c>
-      <c r="C177" t="s">
-        <v>226</v>
+        <v>332</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B178" t="s">
-        <v>336</v>
-      </c>
-      <c r="C178" t="s">
-        <v>226</v>
+        <v>334</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B179" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C179" t="s">
         <v>43</v>
@@ -3830,10 +3831,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B180" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C180" t="s">
         <v>23</v>
@@ -3841,10 +3842,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B181" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C181" t="s">
         <v>43</v>
@@ -3852,21 +3853,21 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B182" t="s">
-        <v>344</v>
-      </c>
-      <c r="C182" t="s">
-        <v>226</v>
+        <v>342</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B183" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C183" t="s">
         <v>43</v>
@@ -3874,10 +3875,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B184" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C184" t="s">
         <v>23</v>
@@ -3885,10 +3886,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B185" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C185" t="s">
         <v>43</v>
@@ -3896,32 +3897,32 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B186" t="s">
-        <v>352</v>
-      </c>
-      <c r="C186" t="s">
-        <v>226</v>
+        <v>350</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B187" t="s">
-        <v>354</v>
-      </c>
-      <c r="C187" t="s">
-        <v>226</v>
+        <v>352</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B188" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C188" t="s">
         <v>23</v>
@@ -3929,10 +3930,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B189" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C189" t="s">
         <v>43</v>
@@ -3940,10 +3941,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B190" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C190" t="s">
         <v>23</v>
@@ -3951,10 +3952,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B191" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C191" t="s">
         <v>23</v>
@@ -3962,10 +3963,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B192" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C192" t="s">
         <v>23</v>
@@ -3973,32 +3974,32 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B193" t="s">
-        <v>366</v>
-      </c>
-      <c r="C193" t="s">
-        <v>226</v>
+        <v>364</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B194" t="s">
-        <v>368</v>
-      </c>
-      <c r="C194" t="s">
-        <v>226</v>
+        <v>366</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B195" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C195" t="s">
         <v>23</v>
@@ -4006,10 +4007,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B196" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C196" t="s">
         <v>23</v>
@@ -4017,21 +4018,21 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B197" t="s">
-        <v>374</v>
-      </c>
-      <c r="C197" t="s">
-        <v>226</v>
+        <v>372</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B198" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C198" t="s">
         <v>43</v>
@@ -4039,10 +4040,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B199" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C199" t="s">
         <v>43</v>
@@ -4050,10 +4051,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B200" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C200" t="s">
         <v>43</v>
@@ -4061,21 +4062,21 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B201" t="s">
-        <v>382</v>
-      </c>
-      <c r="C201" t="s">
-        <v>226</v>
+        <v>380</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B202" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C202" t="s">
         <v>43</v>
@@ -4083,21 +4084,21 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B203" t="s">
-        <v>386</v>
-      </c>
-      <c r="C203" t="s">
-        <v>226</v>
+        <v>384</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B204" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C204" t="s">
         <v>23</v>
@@ -4105,10 +4106,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B205" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C205" t="s">
         <v>43</v>
@@ -4116,10 +4117,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B206" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C206" t="s">
         <v>43</v>
@@ -4127,10 +4128,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B207" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C207" t="s">
         <v>43</v>
@@ -4138,10 +4139,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B208" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C208" t="s">
         <v>43</v>
@@ -4149,10 +4150,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B209" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C209" t="s">
         <v>43</v>
@@ -4160,10 +4161,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B210" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C210" t="s">
         <v>43</v>
@@ -4171,10 +4172,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B211" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C211" t="s">
         <v>43</v>
@@ -4182,10 +4183,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B212" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C212" t="s">
         <v>43</v>
@@ -4193,21 +4194,21 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B213" t="s">
-        <v>405</v>
-      </c>
-      <c r="C213" t="s">
-        <v>226</v>
+        <v>403</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B214" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C214" t="s">
         <v>43</v>
@@ -4215,10 +4216,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B215" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C215" t="s">
         <v>43</v>
@@ -4226,10 +4227,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B216" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C216" t="s">
         <v>43</v>
@@ -4237,10 +4238,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B217" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C217" t="s">
         <v>43</v>
@@ -4248,10 +4249,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B218" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C218" t="s">
         <v>43</v>
@@ -4259,21 +4260,21 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B219" t="s">
-        <v>417</v>
-      </c>
-      <c r="C219" t="s">
-        <v>226</v>
+        <v>415</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B220" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C220" t="s">
         <v>23</v>
@@ -4281,10 +4282,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B221" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C221" t="s">
         <v>43</v>
@@ -4292,10 +4293,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B222" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C222" t="s">
         <v>43</v>
@@ -4303,10 +4304,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B223" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C223" t="s">
         <v>43</v>
@@ -4314,10 +4315,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B224" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C224" t="s">
         <v>23</v>
@@ -4325,10 +4326,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B225" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C225" t="s">
         <v>43</v>
@@ -4336,10 +4337,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B226" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C226" t="s">
         <v>43</v>
@@ -4347,10 +4348,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B227" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C227" t="s">
         <v>43</v>
@@ -4358,10 +4359,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B228" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C228" t="s">
         <v>43</v>
@@ -4369,10 +4370,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B229" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C229" t="s">
         <v>43</v>
@@ -4380,10 +4381,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B230" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C230" t="s">
         <v>43</v>
@@ -4391,10 +4392,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B231" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C231" t="s">
         <v>43</v>
@@ -4402,10 +4403,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B232" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C232" t="s">
         <v>23</v>
@@ -4413,24 +4414,24 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B233" t="s">
-        <v>445</v>
-      </c>
-      <c r="C233" t="s">
-        <v>226</v>
+        <v>443</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B234" t="s">
-        <v>447</v>
-      </c>
-      <c r="C234" t="s">
-        <v>226</v>
+        <v>445</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -4438,167 +4439,168 @@
         <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>448</v>
-      </c>
-      <c r="C235" t="s">
-        <v>226</v>
+        <v>446</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B236" t="s">
-        <v>450</v>
-      </c>
-      <c r="C236" t="s">
-        <v>226</v>
+        <v>448</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B237" t="s">
-        <v>452</v>
-      </c>
-      <c r="C237" t="s">
-        <v>226</v>
+        <v>450</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B238" t="s">
-        <v>454</v>
-      </c>
-      <c r="C238" t="s">
-        <v>226</v>
+        <v>452</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B239" t="s">
-        <v>456</v>
-      </c>
-      <c r="C239" t="s">
-        <v>226</v>
+        <v>454</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B240" t="s">
-        <v>458</v>
-      </c>
-      <c r="C240" t="s">
-        <v>226</v>
+        <v>456</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B241" t="s">
-        <v>460</v>
-      </c>
-      <c r="C241" t="s">
-        <v>226</v>
+        <v>458</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B242" t="s">
-        <v>462</v>
-      </c>
-      <c r="C242" t="s">
-        <v>226</v>
+        <v>460</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B243" t="s">
-        <v>464</v>
-      </c>
-      <c r="C243" t="s">
-        <v>226</v>
+        <v>462</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B244" t="s">
-        <v>466</v>
-      </c>
-      <c r="C244" t="s">
-        <v>226</v>
+        <v>464</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B245" t="s">
-        <v>468</v>
-      </c>
-      <c r="C245" t="s">
-        <v>226</v>
+        <v>466</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B246" t="s">
         <v>3</v>
       </c>
-      <c r="C246" t="s">
-        <v>226</v>
+      <c r="C246" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B247" t="s">
-        <v>471</v>
-      </c>
-      <c r="C247" t="s">
-        <v>226</v>
+        <v>469</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B248" t="s">
-        <v>473</v>
-      </c>
-      <c r="C248" t="s">
-        <v>226</v>
+        <v>471</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B249" t="s">
-        <v>475</v>
-      </c>
-      <c r="C249" t="s">
-        <v>226</v>
+        <v>473</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C249" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
att login e cards
</commit_message>
<xml_diff>
--- a/backend/objetos.xlsx
+++ b/backend/objetos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leozed92-my.sharepoint.com/personal/leozed_leozed92_onmicrosoft_com/Documents/Aplicativos/App GAD SESAU/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EADC58B6-53C8-45BA-8B1C-FBAABA64B35A}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1984CBFD-8D67-4597-84B8-A6AD85781AC0}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="2010" windowWidth="21600" windowHeight="11190" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
+    <workbookView xWindow="-26070" yWindow="2415" windowWidth="21600" windowHeight="11190" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="objetos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="476">
   <si>
     <t>objeto</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>Emergencial</t>
-  </si>
-  <si>
-    <t>0036.051031/2024-05</t>
-  </si>
-  <si>
-    <t>Operação Hospital de Guajará-Mirim</t>
   </si>
   <si>
     <t>0036.059337/2023-11</t>
@@ -1471,6 +1465,9 @@
   </si>
   <si>
     <t>PRESERVAÇÃO DE ÓRGÃOS E CÓRNEAS</t>
+  </si>
+  <si>
+    <t>CONTRATAÇÃO DE EMPRESA ESPECIALIZADA EM SERVIÇOS DE HIGIENIZAÇÃO E LIMPEZA HOSPITALAR E ASSEMELHADAS, LABORATORIAL E AMBULATORIAL - HIGIENIZAÇÃO, CONSERVAÇÃO, DESINFECÇÃO DE SUPERFÍCIES E MOBILIÁRIOS E RECOLHIMENTO INTERNO DOS RESÍDUOS DO GRUPO “D”, VISANDO À OBTENÇÃO DE ADEQUADAS CONDIÇÕES DE SALUBRIDADE E HIGIENE EM DEPENDÊNCIAS DO HOSPITAL REGIONAL DE EXTREMA - HRE, EM CARÁTER EMERGENCIAL, POR UM PERÍODO DE 1 (UM) ANO, OU ATÉ QUE SE CONCLUA O PROCESSO LICITATÓRIO.</t>
   </si>
 </sst>
 </file>
@@ -1533,10 +1530,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1859,7 +1852,7 @@
   <dimension ref="A1:C250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C250"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,18 +1880,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1909,7 +1902,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,7 +1913,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1931,7 +1924,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1942,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1953,7 +1946,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1964,7 +1957,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1975,7 +1968,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1986,7 +1979,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1997,18 +1990,18 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2019,29 +2012,29 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2052,7 +2045,7 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2063,7 +2056,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2074,7 +2067,7 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2085,18 +2078,18 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2107,7 +2100,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2118,7 +2111,7 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2129,7 +2122,7 @@
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2140,7 +2133,7 @@
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2151,7 +2144,7 @@
         <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2162,7 +2155,7 @@
         <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2173,7 +2166,7 @@
         <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2184,7 +2177,7 @@
         <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2195,7 +2188,7 @@
         <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2206,7 +2199,7 @@
         <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2217,7 +2210,7 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2228,7 +2221,7 @@
         <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2239,7 +2232,7 @@
         <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2250,7 +2243,7 @@
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,7 +2254,7 @@
         <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2272,7 +2265,7 @@
         <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,7 +2276,7 @@
         <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2294,7 +2287,7 @@
         <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,7 +2298,7 @@
         <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,7 +2309,7 @@
         <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2327,7 +2320,7 @@
         <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,7 +2331,7 @@
         <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2349,7 +2342,7 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,7 +2353,7 @@
         <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2371,7 +2364,7 @@
         <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,7 +2375,7 @@
         <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,7 +2386,7 @@
         <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,7 +2397,7 @@
         <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2415,7 +2408,7 @@
         <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2426,7 +2419,7 @@
         <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2448,7 +2441,7 @@
         <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2459,7 +2452,7 @@
         <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,7 +2463,7 @@
         <v>113</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,7 +2474,7 @@
         <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2503,7 +2496,7 @@
         <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2514,7 +2507,7 @@
         <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2525,7 +2518,7 @@
         <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,7 +2529,7 @@
         <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2547,7 +2540,7 @@
         <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2558,7 +2551,7 @@
         <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2569,7 +2562,7 @@
         <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2580,7 +2573,7 @@
         <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,29 +2584,29 @@
         <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
         <v>136</v>
       </c>
-      <c r="B67" t="s">
-        <v>137</v>
-      </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
         <v>138</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2624,7 +2617,7 @@
         <v>140</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2635,7 +2628,7 @@
         <v>142</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2646,29 +2639,29 @@
         <v>144</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" t="s">
         <v>145</v>
       </c>
-      <c r="B72" t="s">
-        <v>146</v>
-      </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
         <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2679,7 +2672,7 @@
         <v>149</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2690,7 +2683,7 @@
         <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2701,7 +2694,7 @@
         <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2712,7 +2705,7 @@
         <v>155</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2723,7 +2716,7 @@
         <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2734,21 +2727,21 @@
         <v>159</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>160</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -2756,7 +2749,7 @@
         <v>163</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2767,7 +2760,7 @@
         <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2778,7 +2771,7 @@
         <v>167</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2789,7 +2782,7 @@
         <v>169</v>
       </c>
       <c r="C84" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2800,7 +2793,7 @@
         <v>171</v>
       </c>
       <c r="C85" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2811,7 +2804,7 @@
         <v>173</v>
       </c>
       <c r="C86" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2822,7 +2815,7 @@
         <v>175</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2833,7 +2826,7 @@
         <v>177</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2844,7 +2837,7 @@
         <v>179</v>
       </c>
       <c r="C89" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2855,7 +2848,7 @@
         <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2866,7 +2859,7 @@
         <v>183</v>
       </c>
       <c r="C91" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2877,7 +2870,7 @@
         <v>185</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2888,7 +2881,7 @@
         <v>187</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2899,7 +2892,7 @@
         <v>189</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2910,7 +2903,7 @@
         <v>191</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2921,7 +2914,7 @@
         <v>193</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2932,7 +2925,7 @@
         <v>195</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2943,7 +2936,7 @@
         <v>197</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2954,7 +2947,7 @@
         <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2965,7 +2958,7 @@
         <v>201</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2976,7 +2969,7 @@
         <v>203</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2987,7 +2980,7 @@
         <v>205</v>
       </c>
       <c r="C102" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2998,7 +2991,7 @@
         <v>207</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3009,7 +3002,7 @@
         <v>209</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3013,7 @@
         <v>211</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3053,29 +3046,29 @@
         <v>217</v>
       </c>
       <c r="C108" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>45</v>
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3086,62 +3079,62 @@
         <v>51</v>
       </c>
       <c r="C111" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C112" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C113" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B114" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C114" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C115" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3152,62 +3145,62 @@
         <v>131</v>
       </c>
       <c r="C117" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B118" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C118" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C119" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="B120" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
       <c r="C120" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>204</v>
+        <v>70</v>
       </c>
       <c r="B121" t="s">
-        <v>221</v>
+        <v>71</v>
       </c>
       <c r="C121" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>72</v>
+        <v>220</v>
       </c>
       <c r="B122" t="s">
-        <v>73</v>
+        <v>221</v>
       </c>
       <c r="C122" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3218,7 +3211,7 @@
         <v>223</v>
       </c>
       <c r="C123" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3229,7 +3222,7 @@
         <v>225</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3240,7 +3233,7 @@
         <v>227</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3251,7 +3244,7 @@
         <v>229</v>
       </c>
       <c r="C126" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3262,7 +3255,7 @@
         <v>231</v>
       </c>
       <c r="C127" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3273,7 +3266,7 @@
         <v>233</v>
       </c>
       <c r="C128" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3284,7 +3277,7 @@
         <v>235</v>
       </c>
       <c r="C129" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3295,7 +3288,7 @@
         <v>237</v>
       </c>
       <c r="C130" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3306,7 +3299,7 @@
         <v>239</v>
       </c>
       <c r="C131" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -3317,7 +3310,7 @@
         <v>241</v>
       </c>
       <c r="C132" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -3328,7 +3321,7 @@
         <v>243</v>
       </c>
       <c r="C133" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3339,7 +3332,7 @@
         <v>245</v>
       </c>
       <c r="C134" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3350,7 +3343,7 @@
         <v>247</v>
       </c>
       <c r="C135" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3361,7 +3354,7 @@
         <v>249</v>
       </c>
       <c r="C136" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3372,7 +3365,7 @@
         <v>251</v>
       </c>
       <c r="C137" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -3383,7 +3376,7 @@
         <v>253</v>
       </c>
       <c r="C138" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -3394,7 +3387,7 @@
         <v>255</v>
       </c>
       <c r="C139" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3405,7 +3398,7 @@
         <v>257</v>
       </c>
       <c r="C140" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -3413,18 +3406,18 @@
         <v>258</v>
       </c>
       <c r="B141" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="C141" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>259</v>
+      </c>
+      <c r="B142" t="s">
         <v>260</v>
-      </c>
-      <c r="B142" t="s">
-        <v>237</v>
       </c>
       <c r="C142" t="s">
         <v>3</v>
@@ -3438,18 +3431,18 @@
         <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>3</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>264</v>
+      </c>
+      <c r="B144" t="s">
+        <v>265</v>
+      </c>
+      <c r="C144" t="s">
         <v>263</v>
-      </c>
-      <c r="B144" t="s">
-        <v>264</v>
-      </c>
-      <c r="C144" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3460,7 +3453,7 @@
         <v>267</v>
       </c>
       <c r="C145" t="s">
-        <v>265</v>
+        <v>218</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3471,7 +3464,7 @@
         <v>269</v>
       </c>
       <c r="C146" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3482,7 +3475,7 @@
         <v>271</v>
       </c>
       <c r="C147" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3493,7 +3486,7 @@
         <v>273</v>
       </c>
       <c r="C148" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3504,7 +3497,7 @@
         <v>275</v>
       </c>
       <c r="C149" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3515,7 +3508,7 @@
         <v>277</v>
       </c>
       <c r="C150" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3526,7 +3519,7 @@
         <v>279</v>
       </c>
       <c r="C151" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3537,7 +3530,7 @@
         <v>281</v>
       </c>
       <c r="C152" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3548,7 +3541,7 @@
         <v>283</v>
       </c>
       <c r="C153" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3559,7 +3552,7 @@
         <v>285</v>
       </c>
       <c r="C154" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3570,7 +3563,7 @@
         <v>287</v>
       </c>
       <c r="C155" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3581,7 +3574,7 @@
         <v>289</v>
       </c>
       <c r="C156" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3592,7 +3585,7 @@
         <v>291</v>
       </c>
       <c r="C157" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3603,7 +3596,7 @@
         <v>293</v>
       </c>
       <c r="C158" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3614,7 +3607,7 @@
         <v>295</v>
       </c>
       <c r="C159" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3625,7 +3618,7 @@
         <v>297</v>
       </c>
       <c r="C160" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3636,7 +3629,7 @@
         <v>299</v>
       </c>
       <c r="C161" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3647,7 +3640,7 @@
         <v>301</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3658,7 +3651,7 @@
         <v>303</v>
       </c>
       <c r="C163" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3669,7 +3662,7 @@
         <v>305</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3680,7 +3673,7 @@
         <v>307</v>
       </c>
       <c r="C165" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3691,7 +3684,7 @@
         <v>309</v>
       </c>
       <c r="C166" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3702,7 +3695,7 @@
         <v>311</v>
       </c>
       <c r="C167" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3713,7 +3706,7 @@
         <v>313</v>
       </c>
       <c r="C168" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -3724,7 +3717,7 @@
         <v>315</v>
       </c>
       <c r="C169" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3735,7 +3728,7 @@
         <v>317</v>
       </c>
       <c r="C170" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3746,7 +3739,7 @@
         <v>319</v>
       </c>
       <c r="C171" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3757,7 +3750,7 @@
         <v>321</v>
       </c>
       <c r="C172" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3768,7 +3761,7 @@
         <v>323</v>
       </c>
       <c r="C173" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3779,7 +3772,7 @@
         <v>325</v>
       </c>
       <c r="C174" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3790,7 +3783,7 @@
         <v>327</v>
       </c>
       <c r="C175" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3801,7 +3794,7 @@
         <v>329</v>
       </c>
       <c r="C176" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3812,7 +3805,7 @@
         <v>331</v>
       </c>
       <c r="C177" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3823,7 +3816,7 @@
         <v>333</v>
       </c>
       <c r="C178" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3834,7 +3827,7 @@
         <v>335</v>
       </c>
       <c r="C179" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -3845,7 +3838,7 @@
         <v>337</v>
       </c>
       <c r="C180" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -3856,7 +3849,7 @@
         <v>339</v>
       </c>
       <c r="C181" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -3867,7 +3860,7 @@
         <v>341</v>
       </c>
       <c r="C182" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3878,7 +3871,7 @@
         <v>343</v>
       </c>
       <c r="C183" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3889,7 +3882,7 @@
         <v>345</v>
       </c>
       <c r="C184" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -3900,7 +3893,7 @@
         <v>347</v>
       </c>
       <c r="C185" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -3911,7 +3904,7 @@
         <v>349</v>
       </c>
       <c r="C186" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -3922,7 +3915,7 @@
         <v>351</v>
       </c>
       <c r="C187" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -3933,7 +3926,7 @@
         <v>353</v>
       </c>
       <c r="C188" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3944,7 +3937,7 @@
         <v>355</v>
       </c>
       <c r="C189" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3955,7 +3948,7 @@
         <v>357</v>
       </c>
       <c r="C190" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -3966,7 +3959,7 @@
         <v>359</v>
       </c>
       <c r="C191" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -3977,7 +3970,7 @@
         <v>361</v>
       </c>
       <c r="C192" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -3988,7 +3981,7 @@
         <v>363</v>
       </c>
       <c r="C193" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -3999,7 +3992,7 @@
         <v>365</v>
       </c>
       <c r="C194" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4010,7 +4003,7 @@
         <v>367</v>
       </c>
       <c r="C195" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4021,7 +4014,7 @@
         <v>369</v>
       </c>
       <c r="C196" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -4032,7 +4025,7 @@
         <v>371</v>
       </c>
       <c r="C197" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4043,7 +4036,7 @@
         <v>373</v>
       </c>
       <c r="C198" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4054,7 +4047,7 @@
         <v>375</v>
       </c>
       <c r="C199" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4065,7 +4058,7 @@
         <v>377</v>
       </c>
       <c r="C200" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4076,7 +4069,7 @@
         <v>379</v>
       </c>
       <c r="C201" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4087,7 +4080,7 @@
         <v>381</v>
       </c>
       <c r="C202" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4098,7 +4091,7 @@
         <v>383</v>
       </c>
       <c r="C203" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4109,7 +4102,7 @@
         <v>385</v>
       </c>
       <c r="C204" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4120,7 +4113,7 @@
         <v>387</v>
       </c>
       <c r="C205" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4131,7 +4124,7 @@
         <v>389</v>
       </c>
       <c r="C206" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4139,21 +4132,21 @@
         <v>390</v>
       </c>
       <c r="B207" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C207" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>391</v>
+      </c>
+      <c r="B208" t="s">
         <v>392</v>
       </c>
-      <c r="B208" t="s">
-        <v>391</v>
-      </c>
       <c r="C208" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4164,7 +4157,7 @@
         <v>394</v>
       </c>
       <c r="C209" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4175,7 +4168,7 @@
         <v>396</v>
       </c>
       <c r="C210" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4186,7 +4179,7 @@
         <v>398</v>
       </c>
       <c r="C211" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -4197,7 +4190,7 @@
         <v>400</v>
       </c>
       <c r="C212" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -4208,7 +4201,7 @@
         <v>402</v>
       </c>
       <c r="C213" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -4219,7 +4212,7 @@
         <v>404</v>
       </c>
       <c r="C214" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4230,7 +4223,7 @@
         <v>406</v>
       </c>
       <c r="C215" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -4241,7 +4234,7 @@
         <v>408</v>
       </c>
       <c r="C216" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4252,7 +4245,7 @@
         <v>410</v>
       </c>
       <c r="C217" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4263,7 +4256,7 @@
         <v>412</v>
       </c>
       <c r="C218" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4274,7 +4267,7 @@
         <v>414</v>
       </c>
       <c r="C219" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -4285,7 +4278,7 @@
         <v>416</v>
       </c>
       <c r="C220" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -4296,7 +4289,7 @@
         <v>418</v>
       </c>
       <c r="C221" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4300,7 @@
         <v>420</v>
       </c>
       <c r="C222" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -4318,7 +4311,7 @@
         <v>422</v>
       </c>
       <c r="C223" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -4329,7 +4322,7 @@
         <v>424</v>
       </c>
       <c r="C224" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -4340,7 +4333,7 @@
         <v>426</v>
       </c>
       <c r="C225" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -4351,7 +4344,7 @@
         <v>428</v>
       </c>
       <c r="C226" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -4362,7 +4355,7 @@
         <v>430</v>
       </c>
       <c r="C227" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -4373,7 +4366,7 @@
         <v>432</v>
       </c>
       <c r="C228" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -4384,7 +4377,7 @@
         <v>434</v>
       </c>
       <c r="C229" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -4395,7 +4388,7 @@
         <v>436</v>
       </c>
       <c r="C230" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -4406,7 +4399,7 @@
         <v>438</v>
       </c>
       <c r="C231" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -4417,7 +4410,7 @@
         <v>440</v>
       </c>
       <c r="C232" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -4428,7 +4421,7 @@
         <v>442</v>
       </c>
       <c r="C233" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -4439,7 +4432,7 @@
         <v>444</v>
       </c>
       <c r="C234" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -4450,7 +4443,7 @@
         <v>446</v>
       </c>
       <c r="C235" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -4461,7 +4454,7 @@
         <v>448</v>
       </c>
       <c r="C236" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -4472,7 +4465,7 @@
         <v>450</v>
       </c>
       <c r="C237" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -4483,7 +4476,7 @@
         <v>452</v>
       </c>
       <c r="C238" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -4494,7 +4487,7 @@
         <v>454</v>
       </c>
       <c r="C239" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -4505,7 +4498,7 @@
         <v>456</v>
       </c>
       <c r="C240" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4516,7 +4509,7 @@
         <v>458</v>
       </c>
       <c r="C241" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4527,7 +4520,7 @@
         <v>460</v>
       </c>
       <c r="C242" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4538,7 +4531,7 @@
         <v>462</v>
       </c>
       <c r="C243" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4549,7 +4542,7 @@
         <v>464</v>
       </c>
       <c r="C244" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4560,7 +4553,7 @@
         <v>466</v>
       </c>
       <c r="C245" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4571,7 +4564,7 @@
         <v>468</v>
       </c>
       <c r="C246" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,7 +4575,7 @@
         <v>470</v>
       </c>
       <c r="C247" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -4593,7 +4586,7 @@
         <v>472</v>
       </c>
       <c r="C248" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -4604,18 +4597,18 @@
         <v>474</v>
       </c>
       <c r="C249" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
+        <v>178</v>
+      </c>
+      <c r="B250" t="s">
         <v>475</v>
       </c>
-      <c r="B250" t="s">
-        <v>476</v>
-      </c>
       <c r="C250" t="s">
-        <v>220</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
att diara e relatorio IA
</commit_message>
<xml_diff>
--- a/backend/objetos.xlsx
+++ b/backend/objetos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leozed92-my.sharepoint.com/personal/leozed_leozed92_onmicrosoft_com/Documents/Aplicativos/App GAD SESAU/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1984CBFD-8D67-4597-84B8-A6AD85781AC0}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA33A62D-6FF8-4997-B63A-4D53A3A80BC2}"/>
   <bookViews>
     <workbookView xWindow="-26070" yWindow="2415" windowWidth="21600" windowHeight="11190" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="502">
   <si>
     <t>objeto</t>
   </si>
@@ -1468,6 +1468,84 @@
   </si>
   <si>
     <t>CONTRATAÇÃO DE EMPRESA ESPECIALIZADA EM SERVIÇOS DE HIGIENIZAÇÃO E LIMPEZA HOSPITALAR E ASSEMELHADAS, LABORATORIAL E AMBULATORIAL - HIGIENIZAÇÃO, CONSERVAÇÃO, DESINFECÇÃO DE SUPERFÍCIES E MOBILIÁRIOS E RECOLHIMENTO INTERNO DOS RESÍDUOS DO GRUPO “D”, VISANDO À OBTENÇÃO DE ADEQUADAS CONDIÇÕES DE SALUBRIDADE E HIGIENE EM DEPENDÊNCIAS DO HOSPITAL REGIONAL DE EXTREMA - HRE, EM CARÁTER EMERGENCIAL, POR UM PERÍODO DE 1 (UM) ANO, OU ATÉ QUE SE CONCLUA O PROCESSO LICITATÓRIO.</t>
+  </si>
+  <si>
+    <t>FORNECIMENTO CONTÍNUO DE REAGENTE PARA DIAGNÓSTICO CLÍNICO, TIPO CONJUNTO COMPLETO PARA AUTOMAÇÃO, PARA ANÁLISE QUANTITATIVA DE GASOMETRIA, COM FORNECIMENTO DE EQUIPAMENTOS (GASÔMETROS) EM REGIME DE COMODATO</t>
+  </si>
+  <si>
+    <t>0036.029392/2025-48</t>
+  </si>
+  <si>
+    <t>aquisição de serviços de coffee break - SESMT</t>
+  </si>
+  <si>
+    <t>0036.017399/2025-17</t>
+  </si>
+  <si>
+    <t>medicamento classe de INJETAVEIS III</t>
+  </si>
+  <si>
+    <t>0063.001173/2025-77</t>
+  </si>
+  <si>
+    <t>Locação de clinica odontologica estruturada - POC</t>
+  </si>
+  <si>
+    <t>0036.025786/2025-27</t>
+  </si>
+  <si>
+    <t>Aquisição de medicamentos Grandes Volumes</t>
+  </si>
+  <si>
+    <t>0036.030292/2025-64</t>
+  </si>
+  <si>
+    <t>Solução de Hemodiálise</t>
+  </si>
+  <si>
+    <t>0036.029730/2025-41</t>
+  </si>
+  <si>
+    <t>Manutenção preventiva e corretiva em condicionadores de ar com fornecimento e reposição de peças, acessórios e componentes eletrônicos do Sistema de Climatização - HRSFG</t>
+  </si>
+  <si>
+    <t>0036.021034/2025-97</t>
+  </si>
+  <si>
+    <t>Prestação de Serviço de ANESTESIOLOGISTA</t>
+  </si>
+  <si>
+    <t>0036.027285/2025-85</t>
+  </si>
+  <si>
+    <t>Aquisição de bombas pressurizadoras, modelo SCALA1 3-35 (ou similar compatível com o sistema HEURO) do sistema de tratamento de água para hemodiálise da Unidade de Terapia Intensiva UTI</t>
+  </si>
+  <si>
+    <t>0036.014122/2025-32</t>
+  </si>
+  <si>
+    <t>ÁGUA MINERAL GARRAFÃO RETORNÁVEL DE 20 LITROS, ÁGUA MINERAL SEM GÁS DE 500ML E ÁGUA MINERAL COM GÁS DE 500ML, para atender as demandas das unidades do interior</t>
+  </si>
+  <si>
+    <t>0036.026848/2025-18</t>
+  </si>
+  <si>
+    <t>Aquisição de soluções parenterais estéreis (soros), especificamente Glicose nas apresentações de 250 mL e 500 ml</t>
+  </si>
+  <si>
+    <t>Adesão à Ata</t>
+  </si>
+  <si>
+    <t>0036.030151/2025-41</t>
+  </si>
+  <si>
+    <t>prestação de limpeza, conservação, higienização e desinfecção com fornecimento de materiais e equipamentos - GRS4</t>
+  </si>
+  <si>
+    <t>0036.027016/2025-19</t>
+  </si>
+  <si>
+    <t>SERVIÇOS DE EXAMES LABORATORIAIS - HRE</t>
   </si>
 </sst>
 </file>
@@ -1530,6 +1608,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}">
-  <dimension ref="A1:C250"/>
+  <dimension ref="A1:C263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,6 +4693,128 @@
         <v>3</v>
       </c>
     </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>254</v>
+      </c>
+      <c r="B251" t="s">
+        <v>476</v>
+      </c>
+      <c r="C251" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>477</v>
+      </c>
+      <c r="B252" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>479</v>
+      </c>
+      <c r="B253" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>481</v>
+      </c>
+      <c r="B254" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>483</v>
+      </c>
+      <c r="B255" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>485</v>
+      </c>
+      <c r="B256" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>487</v>
+      </c>
+      <c r="B257" t="s">
+        <v>488</v>
+      </c>
+      <c r="C257" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>489</v>
+      </c>
+      <c r="B258" t="s">
+        <v>490</v>
+      </c>
+      <c r="C258" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>491</v>
+      </c>
+      <c r="B259" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>493</v>
+      </c>
+      <c r="B260" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>495</v>
+      </c>
+      <c r="B261" t="s">
+        <v>496</v>
+      </c>
+      <c r="C261" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>498</v>
+      </c>
+      <c r="B262" t="s">
+        <v>499</v>
+      </c>
+      <c r="C262" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>500</v>
+      </c>
+      <c r="B263" t="s">
+        <v>501</v>
+      </c>
+      <c r="C263" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C249" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização automática dos scripts ETL
</commit_message>
<xml_diff>
--- a/backend/objetos.xlsx
+++ b/backend/objetos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leozed92-my.sharepoint.com/personal/leozed_leozed92_onmicrosoft_com/Documents/Aplicativos/App GAD SESAU/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E53BFC-0421-4058-BB54-09E7008B3771}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{C24DD8E0-50BB-40E4-B648-E8FAFBB74FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{595341F3-CC78-4EDD-A32A-3B9CE51153A8}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11190" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{92D8D400-3915-4B7A-B5E9-ACA32B0E4BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="objetos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="529">
   <si>
     <t>objeto</t>
   </si>
@@ -1570,6 +1570,63 @@
   </si>
   <si>
     <t>medicamentos, Soluções orais II</t>
+  </si>
+  <si>
+    <t>0036.024403/2025-01</t>
+  </si>
+  <si>
+    <t>medicamentos Soluções orais I</t>
+  </si>
+  <si>
+    <t>0036.033486/2025-11</t>
+  </si>
+  <si>
+    <t>Alimentação Hospitalar - HBAP, HICD, CEMETRON, CRUE, CEREL.</t>
+  </si>
+  <si>
+    <t>0036.033230/2025-12</t>
+  </si>
+  <si>
+    <t>Fornecimento de alimentação hospitalar - HRC, HEURO</t>
+  </si>
+  <si>
+    <t>0036.032746/2025-31</t>
+  </si>
+  <si>
+    <t>prestação de serviços de locação de Módulos/Centrais de Compressores de Ar Medicinal - HEPSJP-II.</t>
+  </si>
+  <si>
+    <t>0036.032361/2025-74</t>
+  </si>
+  <si>
+    <t>0036.020064/2025-86</t>
+  </si>
+  <si>
+    <t>GCET - Gerência de Coordenação Estadual de Transplantes. Bolsa Plástica estéril para acondicionamento e isolamento de órgãos</t>
+  </si>
+  <si>
+    <t>0036.023632/2025-09</t>
+  </si>
+  <si>
+    <t>Engenharia Clínica,Serviço de Gerenciamento de Equipamentos Manutenção Corretiva, Preventiva, Preditiva e Calibração dos Equipamentos com Reposição de Peças e Acessórios, Serviço de Gerenciamento de Equipamentos Manutenção Corretiva, Preventiva, Preditiva e Calibração dos Equipamentos com Reposição de Peças e Acessórios - POC</t>
+  </si>
+  <si>
+    <t>0036.027089/2025-19</t>
+  </si>
+  <si>
+    <t>serviços de manutenção preventiva e corretiva em condicionadores de ar (com fornecimento e reposição de peças, acessórios e componentes eletrônicos) para as unidades administrativa</t>
+  </si>
+  <si>
+    <t>0036.017198/2025-10</t>
+  </si>
+  <si>
+    <t>Emergencial - serviços de neurologia Cirúrgica e Neurologia Clínica</t>
+  </si>
+  <si>
+    <t>0036.016942/2024-88</t>
+  </si>
+  <si>
+    <t>Construção de um Espaço de convivência - POC</t>
   </si>
 </sst>
 </file>
@@ -1632,10 +1689,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1955,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}">
-  <dimension ref="A1:C267"/>
+  <dimension ref="A1:C277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C267"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4877,6 +4930,107 @@
         <v>509</v>
       </c>
     </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>510</v>
+      </c>
+      <c r="B268" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>512</v>
+      </c>
+      <c r="B269" t="s">
+        <v>513</v>
+      </c>
+      <c r="C269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>514</v>
+      </c>
+      <c r="B270" t="s">
+        <v>515</v>
+      </c>
+      <c r="C270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>516</v>
+      </c>
+      <c r="B271" t="s">
+        <v>517</v>
+      </c>
+      <c r="C271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>518</v>
+      </c>
+      <c r="B272" t="s">
+        <v>515</v>
+      </c>
+      <c r="C272" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>519</v>
+      </c>
+      <c r="B273" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>521</v>
+      </c>
+      <c r="B274" t="s">
+        <v>522</v>
+      </c>
+      <c r="C274" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>523</v>
+      </c>
+      <c r="B275" t="s">
+        <v>524</v>
+      </c>
+      <c r="C275" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>525</v>
+      </c>
+      <c r="B276" t="s">
+        <v>526</v>
+      </c>
+      <c r="C276" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>527</v>
+      </c>
+      <c r="B277" t="s">
+        <v>528</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C249" xr:uid="{4A2FF0CA-3C4D-4BFF-9AA5-A0CFD76751B1}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>